<commit_message>
Excel add IsConveyor Formula
Signed-off-by: EmanueleAlfano <e.alfano@automatesrl.it>
</commit_message>
<xml_diff>
--- a/parametricExcel-Model.xlsx
+++ b/parametricExcel-Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaScipioni\Desktop\A_ZURIGO\GIT_repo\tiaToolsAutomate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmanueleAlfano\Documents\01_Projects\GitRepo\automateUtility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EB10F9-CBC2-4843-8E43-CF957E3F70E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FD4D52-F794-41B9-AEE7-8C29496B1740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="817" xr2:uid="{2DAA8C73-5A0F-48AB-96BD-6422EDFEC170}"/>
+    <workbookView xWindow="28680" yWindow="-9105" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{2DAA8C73-5A0F-48AB-96BD-6422EDFEC170}"/>
   </bookViews>
   <sheets>
     <sheet name="Conveiur-utenza" sheetId="6" r:id="rId1"/>
@@ -722,9 +722,6 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -796,6 +793,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -839,7 +839,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{30787362-D8AD-4BFD-B40F-A0CE2FC5D120}" name="Tabella5" displayName="Tabella5" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{30787362-D8AD-4BFD-B40F-A0CE2FC5D120}" name="Tabella5" displayName="Tabella5" ref="A1:J2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:J2" xr:uid="{30787362-D8AD-4BFD-B40F-A0CE2FC5D120}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E0A71EBF-B751-48D3-B49F-BC48043FCF32}" name="conv" dataDxfId="16"/>
@@ -848,12 +848,12 @@
     <tableColumn id="7" xr3:uid="{C1FEE6D8-1DB3-4062-A1D8-1001D25C54F7}" name="Linea" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{746C70D6-68B6-4B0C-B0CE-91076476A5CB}" name="tipo" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{924EEFB3-CCD3-4D9A-B637-2B699BB383E6}" name="Daisy Chain MCP" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{102EB18A-8C02-4213-88EE-1E8AB5A478A0}" name="Daisy Chain CAL" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{852AF5FF-8971-447E-A4C1-39AE0B24FAE5}" name="PCT" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{2F9F6B43-94FA-4277-BB96-D48C76ED67A9}" name="IsConveyor" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{102EB18A-8C02-4213-88EE-1E8AB5A478A0}" name="Daisy Chain CAL" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{852AF5FF-8971-447E-A4C1-39AE0B24FAE5}" name="PCT" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{2F9F6B43-94FA-4277-BB96-D48C76ED67A9}" name="IsConveyor" dataDxfId="8">
       <calculatedColumnFormula>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),FALSE,IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{988A770F-D589-4748-93E6-DCE0AB2C9888}" name="Id_Obj" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{988A770F-D589-4748-93E6-DCE0AB2C9888}" name="Id_Obj" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1207,7 +1207,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="33" t="b">
+        <f>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),FALSE,IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1556,29 +1561,29 @@
     <mergeCell ref="H2:T2"/>
   </mergeCells>
   <conditionalFormatting sqref="AE3">
-    <cfRule type="containsText" dxfId="7" priority="191" operator="containsText" text="DIVERSO">
+    <cfRule type="containsText" dxfId="6" priority="191" operator="containsText" text="DIVERSO">
       <formula>NOT(ISERROR(SEARCH("DIVERSO",AE3)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="192" operator="equal">
       <formula>"""DIVERSO"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="193" operator="equal">
       <formula>"""DIVERSO"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AE1048576">
-    <cfRule type="containsText" dxfId="4" priority="86" operator="containsText" text="1234">
+    <cfRule type="containsText" dxfId="3" priority="86" operator="containsText" text="1234">
       <formula>NOT(ISERROR(SEARCH("1234",AE4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="160" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="2" priority="160" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",AE4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="duplicateValues" dxfId="2" priority="200"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="200"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="201"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="201"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Excel is conveyor formula update to include launch conveyor in merge
Signed-off-by: EmanueleAlfano <e.alfano@automatesrl.it>
</commit_message>
<xml_diff>
--- a/parametricExcel-Model.xlsx
+++ b/parametricExcel-Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmanueleAlfano\Documents\01_Projects\GitRepo\automateUtility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FD4D52-F794-41B9-AEE7-8C29496B1740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03F065-7FDE-4F1A-BA4B-B319B0C9287D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9105" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{2DAA8C73-5A0F-48AB-96BD-6422EDFEC170}"/>
   </bookViews>
@@ -851,7 +851,7 @@
     <tableColumn id="10" xr3:uid="{102EB18A-8C02-4213-88EE-1E8AB5A478A0}" name="Daisy Chain CAL" dataDxfId="10"/>
     <tableColumn id="6" xr3:uid="{852AF5FF-8971-447E-A4C1-39AE0B24FAE5}" name="PCT" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{2F9F6B43-94FA-4277-BB96-D48C76ED67A9}" name="IsConveyor" dataDxfId="8">
-      <calculatedColumnFormula>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),FALSE,IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),IF(Tabella5[[#This Row],[tipo]]="MERGE",TRUE,FALSE),IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{988A770F-D589-4748-93E6-DCE0AB2C9888}" name="Id_Obj" dataDxfId="7"/>
   </tableColumns>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="33" t="b">
-        <f>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),FALSE,IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</f>
+        <f>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),IF(Tabella5[[#This Row],[tipo]]="MERGE",TRUE,FALSE),IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
aggiornamento xr model appoggio excel
Signed-off-by: windex2022 <e.scipioni@automasrl.it>
</commit_message>
<xml_diff>
--- a/parametricExcel-Model.xlsx
+++ b/parametricExcel-Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmanueleAlfano\Documents\01_Projects\GitRepo\automateUtility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaScipioni\Desktop\A_ZURIGO\GIT_repo\tiaToolsAutomate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A03F065-7FDE-4F1A-BA4B-B319B0C9287D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB26905-F0B5-4931-97AC-79FDECA7BA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9105" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{2DAA8C73-5A0F-48AB-96BD-6422EDFEC170}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{2DAA8C73-5A0F-48AB-96BD-6422EDFEC170}"/>
   </bookViews>
   <sheets>
     <sheet name="Conveiur-utenza" sheetId="6" r:id="rId1"/>
@@ -851,7 +851,7 @@
     <tableColumn id="10" xr3:uid="{102EB18A-8C02-4213-88EE-1E8AB5A478A0}" name="Daisy Chain CAL" dataDxfId="10"/>
     <tableColumn id="6" xr3:uid="{852AF5FF-8971-447E-A4C1-39AE0B24FAE5}" name="PCT" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{2F9F6B43-94FA-4277-BB96-D48C76ED67A9}" name="IsConveyor" dataDxfId="8">
-      <calculatedColumnFormula>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),IF(Tabella5[[#This Row],[tipo]]="MERGE",TRUE,FALSE),IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),IF(Tabella5[[#This Row],[tipo]]="MERGE",TRUE,IF(Tabella5[[#This Row],[tipo]]="XR",TRUE,FALSE)),IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{988A770F-D589-4748-93E6-DCE0AB2C9888}" name="Id_Obj" dataDxfId="7"/>
   </tableColumns>
@@ -1159,23 +1159,23 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="33" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="33" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" style="33" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="33" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="33" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
@@ -1207,13 +1207,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I2" s="33" t="b">
-        <f>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),IF(Tabella5[[#This Row],[tipo]]="MERGE",TRUE,FALSE),IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</f>
+        <f>IF(ISERROR(FIND("CONVEYOR",Tabella5[[#This Row],[tipo]])),IF(Tabella5[[#This Row],[tipo]]="MERGE",TRUE,IF(Tabella5[[#This Row],[tipo]]="XR",TRUE,FALSE)),IF(AND(ISERROR(FIND("FB",Tabella5[[#This Row],[conv]])),ISERROR(FIND("ME",Tabella5[[#This Row],[conv]]))),FALSE,TRUE))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1232,45 +1232,45 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="38" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="9.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="52.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="9.140625" style="2" hidden="1" customWidth="1"/>
     <col min="17" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="2"/>
-    <col min="21" max="21" width="14.33203125" style="34" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="2.6640625" style="34" customWidth="1"/>
-    <col min="23" max="23" width="2.6640625" style="15" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="2"/>
+    <col min="21" max="21" width="14.28515625" style="34" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" style="34" customWidth="1"/>
+    <col min="23" max="23" width="2.7109375" style="15" customWidth="1"/>
     <col min="24" max="24" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.6640625" style="15" customWidth="1"/>
-    <col min="26" max="26" width="44.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.7109375" style="15" customWidth="1"/>
+    <col min="26" max="26" width="44.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="64" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="2.6640625" style="15" customWidth="1"/>
-    <col min="31" max="31" width="12.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="2.6640625" style="15" customWidth="1"/>
+    <col min="30" max="30" width="2.7109375" style="15" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="2.7109375" style="15" customWidth="1"/>
     <col min="33" max="33" width="38" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="58.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="1.6640625" customWidth="1"/>
-    <col min="40" max="40" width="1.6640625" style="32" customWidth="1"/>
-    <col min="41" max="41" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="58.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="1.7109375" customWidth="1"/>
+    <col min="40" max="40" width="1.7109375" style="32" customWidth="1"/>
+    <col min="41" max="41" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>13</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="AJ1" s="25"/>
       <c r="AN1" s="31"/>
     </row>
-    <row r="2" spans="1:40" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
         <v>17</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="AJ2" s="25"/>
       <c r="AN2" s="31"/>
     </row>
-    <row r="3" spans="1:40" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>19</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>51</v>
       </c>

</xml_diff>